<commit_message>
Sistemata gerarchia con parametri livello e rarita a parte
</commit_message>
<xml_diff>
--- a/ProvaCombina.xlsx
+++ b/ProvaCombina.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\OneDrive\Documenti\Universitas\INFORMATICA\II Anno\Programmazione ad oggetti\2017\oop_project\MasterBranch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23746b98e795164b/Documenti/Universitas/INFORMATICA/II Anno/Programmazione ad oggetti/2017/oop_project/MasterBranch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="A2A2EAA0EA2ED2C453EDC1BDB73A7BBEBAD11999" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{78C0F777-B045-4F5E-9C3C-9B0E534D7FF0}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="A2A2EAA0EA2ED2C453EDC1BDB73A7BBEBAD11999" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{7CDAD58D-B110-4087-A768-C30A19579A44}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="18514" windowHeight="8057" xr2:uid="{1F8DE007-AF5C-4635-9AC8-17D62945ABE5}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="12343" windowHeight="6257" xr2:uid="{1F8DE007-AF5C-4635-9AC8-17D62945ABE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>oggettoA.combina(oggettoB)</t>
   </si>
@@ -60,9 +60,6 @@
     <t>spirito</t>
   </si>
   <si>
-    <t>SommeDirette</t>
-  </si>
-  <si>
     <t>ErbaNuovo</t>
   </si>
   <si>
@@ -82,13 +79,28 @@
   </si>
   <si>
     <t>ManaCristallo</t>
+  </si>
+  <si>
+    <t>Percentuali</t>
+  </si>
+  <si>
+    <t>PuntiVita</t>
+  </si>
+  <si>
+    <t>livello</t>
+  </si>
+  <si>
+    <t>MediaPercentuali</t>
+  </si>
+  <si>
+    <t>ErbaNormalizzato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +110,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -217,17 +221,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -542,108 +548,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442DADB5-51D4-4365-AA3E-E89CE9D4231D}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.921875" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.23046875" style="3"/>
-    <col min="3" max="3" width="22.921875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="22.765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="3"/>
-    <col min="7" max="7" width="23.07421875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.23046875" style="3"/>
+    <col min="3" max="3" width="14.53515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.921875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="22.765625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="9.23046875" style="3"/>
+    <col min="9" max="9" width="23.07421875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.23046875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="C2" s="13"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="21">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="21">
+        <v>5</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17">
-        <v>5</v>
-      </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="10">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10">
+        <f>B4*B$3/E$4</f>
+        <v>0.48</v>
+      </c>
+      <c r="D4" s="3">
+        <f>(C4+H4)/2</f>
+        <v>0.29172413793103447</v>
+      </c>
+      <c r="E4" s="9">
+        <f>SUM(B4:B6)*B3</f>
         <v>25</v>
       </c>
-      <c r="D4" s="9">
-        <f>SUM(B4:B6)*B3</f>
-        <v>125</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11">
-        <v>4</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="1">
-        <f>SUM(F4:F6)*F3</f>
-        <v>670</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F4" s="9"/>
+      <c r="G4" s="11">
+        <v>15</v>
+      </c>
+      <c r="H4" s="11">
+        <f>G4*G$3/J$4</f>
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="1">
+        <f>SUM(G4:G6)*G3</f>
+        <v>725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="10">
-        <v>100</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="C5" s="10">
+        <f>B5*B$3/E$4</f>
+        <v>0.52</v>
+      </c>
+      <c r="D5" s="3">
+        <f>(C5+H6+H7)/2</f>
+        <v>0.74620689655172412</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -651,13 +687,18 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="11">
+      <c r="F6" s="9"/>
+      <c r="G6" s="11">
         <v>130</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H6" s="11">
+        <f>G6*G$3/J$4</f>
+        <v>0.89655172413793105</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -665,13 +706,18 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="11">
-        <v>12</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F7" s="9"/>
+      <c r="G7" s="11">
+        <v>11</v>
+      </c>
+      <c r="H7" s="11">
+        <f>G7*G$3/J$4</f>
+        <v>7.586206896551724E-2</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -679,139 +725,204 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3">
         <f>B3</f>
         <v>1</v>
       </c>
-      <c r="E11" s="3">
-        <f>B11*SUM(C12:C13)</f>
-        <v>855</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <f>(B11+B12)*B10</f>
+        <v>777.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <f>(B4*B3+D4*J4)/B3</f>
+        <v>223.5</v>
+      </c>
+      <c r="C11" s="9">
+        <f>B11*E12</f>
+        <v>43.118971061093248</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="9">
-        <f>B4*B$3 + F$3*F4</f>
-        <v>45</v>
-      </c>
-      <c r="C12" s="3">
-        <f>B12/B$11</f>
-        <v>45</v>
-      </c>
-      <c r="D12" s="3">
-        <f>C12*E$13</f>
-        <v>7.8947368421052628</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="9">
-        <f>(F6+F7)*F3+B5*B3</f>
-        <v>810</v>
-      </c>
-      <c r="C13" s="3">
-        <f>B13/B$11</f>
-        <v>810</v>
-      </c>
-      <c r="D13" s="22">
-        <f>C13*E$13</f>
-        <v>142.10526315789474</v>
-      </c>
-      <c r="E13" s="3">
-        <f>H13/E11</f>
-        <v>0.17543859649122806</v>
-      </c>
-      <c r="G13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <f>(B5*B3+D5*J4)/B3</f>
+        <v>554</v>
+      </c>
+      <c r="C12" s="9">
+        <f>B12*E12</f>
+        <v>106.88102893890675</v>
+      </c>
+      <c r="E12" s="3">
+        <f>J13*B10/E10</f>
+        <v>0.19292604501607716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="C13" s="9"/>
+      <c r="I13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="3">
+      <c r="J13" s="3">
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="4"/>
       <c r="B14" s="9"/>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="C14" s="9"/>
+      <c r="I14" s="3">
         <v>2</v>
       </c>
-      <c r="H14" s="3">
-        <f>H$13*G14</f>
+      <c r="J14" s="3">
+        <f>J$13*I14</f>
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="4"/>
-      <c r="E15" s="3">
-        <f>SUM(D12:D13)*B11</f>
-        <v>150</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="I15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="3">
-        <f t="shared" ref="H15:H16" si="0">H$13*G15</f>
+      <c r="J15" s="3">
+        <f t="shared" ref="J15:J16" si="0">J$13*I15</f>
         <v>450</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="4"/>
-      <c r="G16" s="3">
+      <c r="I16" s="3">
         <v>4</v>
       </c>
-      <c r="H16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="4"/>
-      <c r="G17" s="9">
+      <c r="I17" s="9">
         <v>5</v>
       </c>
-      <c r="H17" s="3">
-        <f>H$13*G17</f>
+      <c r="J17" s="3">
+        <f>J$13*I17</f>
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <f>B19*SUM(D20:D21)</f>
+        <v>805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B4*B$3 + G$3*G4</f>
+        <v>87</v>
+      </c>
+      <c r="D20" s="3">
+        <f>B20/B$19</f>
+        <v>87</v>
+      </c>
+      <c r="E20" s="3">
+        <f>D20*F$21</f>
+        <v>16.211180124223603</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9">
+        <f>(G6+G7)*G3+B5*B3</f>
+        <v>718</v>
+      </c>
+      <c r="D21" s="3">
+        <f>B21/B$19</f>
+        <v>718</v>
+      </c>
+      <c r="E21" s="19">
+        <f>D21*F$21</f>
+        <v>133.7888198757764</v>
+      </c>
+      <c r="F21" s="3">
+        <f>J13/F19</f>
+        <v>0.18633540372670807</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F23" s="3">
+        <f>SUM(E20:E21)*B19</f>
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
ProvaCombina aggiornato con test coerente col main
</commit_message>
<xml_diff>
--- a/ProvaCombina.xlsx
+++ b/ProvaCombina.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23746b98e795164b/Documenti/Universitas/INFORMATICA/II Anno/Programmazione ad oggetti/2017/oop_project/MasterBranch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="A2A2EAA0EA2ED2C453EDC1BDB73A7BBEBAD11999" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{7CDAD58D-B110-4087-A768-C30A19579A44}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="A2A2EAA0EA2ED2C453EDC1BDB73A7BBEBAD11999" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{E3C4CCB2-508F-46EA-8155-AAADF86F632B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="12343" windowHeight="6257" xr2:uid="{1F8DE007-AF5C-4635-9AC8-17D62945ABE5}"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="12343" windowHeight="6257" activeTab="1" xr2:uid="{1F8DE007-AF5C-4635-9AC8-17D62945ABE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>oggettoA.combina(oggettoB)</t>
   </si>
@@ -94,6 +95,30 @@
   </si>
   <si>
     <t>ErbaNormalizzato</t>
+  </si>
+  <si>
+    <t>Rarita</t>
+  </si>
+  <si>
+    <t>ManaTot</t>
+  </si>
+  <si>
+    <t>Pietra</t>
+  </si>
+  <si>
+    <t>attacco</t>
+  </si>
+  <si>
+    <t>rarita</t>
+  </si>
+  <si>
+    <t>NuovaPietra</t>
+  </si>
+  <si>
+    <t>MediePerc</t>
+  </si>
+  <si>
+    <t>Normalizzato</t>
   </si>
 </sst>
 </file>
@@ -204,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -231,6 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442DADB5-51D4-4365-AA3E-E89CE9D4231D}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -568,15 +594,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="18"/>
       <c r="I1" s="2"/>
     </row>
@@ -637,7 +663,7 @@
       </c>
       <c r="D4" s="3">
         <f>(C4+H4)/2</f>
-        <v>0.29172413793103447</v>
+        <v>0.24381679389312977</v>
       </c>
       <c r="E4" s="9">
         <f>SUM(B4:B6)*B3</f>
@@ -645,16 +671,16 @@
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="11">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H4" s="11">
         <f>G4*G$3/J$4</f>
-        <v>0.10344827586206896</v>
+        <v>7.6335877862595417E-3</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="1">
         <f>SUM(G4:G6)*G3</f>
-        <v>725</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -670,7 +696,7 @@
       </c>
       <c r="D5" s="3">
         <f>(C5+H6+H7)/2</f>
-        <v>0.74620689655172412</v>
+        <v>0.79816793893129778</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -693,7 +719,7 @@
       </c>
       <c r="H6" s="11">
         <f>G6*G$3/J$4</f>
-        <v>0.89655172413793105</v>
+        <v>0.99236641221374045</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -712,7 +738,7 @@
       </c>
       <c r="H7" s="11">
         <f>G7*G$3/J$4</f>
-        <v>7.586206896551724E-2</v>
+        <v>8.3969465648854963E-2</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="12"/>
@@ -759,7 +785,7 @@
       </c>
       <c r="E10" s="3">
         <f>(B11+B12)*B10</f>
-        <v>777.5</v>
+        <v>707.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
@@ -768,11 +794,11 @@
       </c>
       <c r="B11" s="3">
         <f>(B4*B3+D4*J4)/B3</f>
-        <v>223.5</v>
+        <v>171.7</v>
       </c>
       <c r="C11" s="9">
         <f>B11*E12</f>
-        <v>43.118971061093248</v>
+        <v>36.402826855123671</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>13</v>
@@ -784,15 +810,15 @@
       </c>
       <c r="B12" s="3">
         <f>(B5*B3+D5*J4)/B3</f>
-        <v>554</v>
+        <v>535.80000000000007</v>
       </c>
       <c r="C12" s="9">
         <f>B12*E12</f>
-        <v>106.88102893890675</v>
+        <v>113.59717314487635</v>
       </c>
       <c r="E12" s="3">
         <f>J13*B10/E10</f>
-        <v>0.19292604501607716</v>
+        <v>0.21201413427561838</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -865,7 +891,7 @@
       </c>
       <c r="F19" s="3">
         <f>B19*SUM(D20:D21)</f>
-        <v>805</v>
+        <v>735</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
@@ -874,15 +900,15 @@
       </c>
       <c r="B20" s="9">
         <f>B4*B$3 + G$3*G4</f>
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="D20" s="3">
         <f>B20/B$19</f>
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3">
         <f>D20*F$21</f>
-        <v>16.211180124223603</v>
+        <v>3.4693877551020407</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>13</v>
@@ -902,11 +928,11 @@
       </c>
       <c r="E21" s="19">
         <f>D21*F$21</f>
-        <v>133.7888198757764</v>
+        <v>146.53061224489795</v>
       </c>
       <c r="F21" s="3">
         <f>J13/F19</f>
-        <v>0.18633540372670807</v>
+        <v>0.20408163265306123</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
@@ -927,4 +953,270 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63D10B5-802B-4845-89B2-508C48F2305C}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="4" width="11.53515625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>SUM(B3:B6)*B2</f>
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f>SUM(F3:F7)*F2</f>
+        <v>710</v>
+      </c>
+      <c r="K2">
+        <f>1135/5</f>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <f>B3*B$2/C$2</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="D3">
+        <f>(C3+G3)/2</f>
+        <v>0.15285832642916322</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f>F3*F$2/G$2</f>
+        <v>7.0422535211267609E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C6" si="0">B4*B$2/C$2</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D6" si="1">(C4+G4)/2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="2">F4*F$2/G$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.22908036454018227</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.28169014084507044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0.30115990057995029</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1.4084507042253521E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.63380281690140849</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>SUM(B11:B14)</f>
+        <v>570</v>
+      </c>
+      <c r="D10">
+        <f>150*B10/C10</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="E10">
+        <f>SUM(D11:D14)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>B3*B$2+D3*G$2</f>
+        <v>128.52941176470588</v>
+      </c>
+      <c r="D11">
+        <f>D$10*B11</f>
+        <v>33.823529411764703</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:B14" si="3">B4*B$2+C4*G$2</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D14" si="4">D$10*B12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <f>B5*B$2+D5*G$2</f>
+        <v>177.64705882352942</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="4"/>
+        <v>46.749226006191947</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f>B6*B$2+D6*G$2</f>
+        <v>263.8235294117647</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="4"/>
+        <v>69.427244582043343</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>